<commit_message>
Issue fixes from master branch
</commit_message>
<xml_diff>
--- a/src/test/resources/IngredientsAndComorbidities-ScrapperHackathon.xlsx
+++ b/src/test/resources/IngredientsAndComorbidities-ScrapperHackathon.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anil.basudkar\eclipse-workspace\StarTechiesScraping\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8e957e20673ddefa/Desktop/workspace_numppy_new/StarTechiesScraping/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44A302E-3A04-43F7-862F-C300228EB62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{C44A302E-3A04-43F7-862F-C300228EB62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76737A4F-F6AC-4102-B311-0BEC7F15C5B9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diabetes-Hypothyroidism-Hyperte" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="Final list for LFV Elimination " sheetId="2" r:id="rId2"/>
+    <sheet name="LFVElimination" sheetId="2" r:id="rId2"/>
     <sheet name="LCHFElimination" sheetId="3" r:id="rId3"/>
     <sheet name="Filter -1 Allergies - Bonus Poi" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -1511,6 +1511,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -1718,15 +1722,15 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="23.90625" customWidth="1"/>
-    <col min="3" max="4" width="22.6328125" customWidth="1"/>
-    <col min="5" max="5" width="26.36328125" customWidth="1"/>
+    <col min="1" max="2" width="23.88671875" customWidth="1"/>
+    <col min="3" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" customWidth="1"/>
     <col min="6" max="6" width="30" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="20.08984375" customWidth="1"/>
-    <col min="9" max="26" width="14.453125" customWidth="1"/>
+    <col min="8" max="8" width="20.109375" customWidth="1"/>
+    <col min="9" max="26" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.5" customHeight="1">
@@ -30050,20 +30054,20 @@
   </sheetPr>
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="40.36328125" customWidth="1"/>
-    <col min="2" max="2" width="24.36328125" customWidth="1"/>
-    <col min="3" max="3" width="34.36328125" customWidth="1"/>
-    <col min="4" max="4" width="25.36328125" customWidth="1"/>
-    <col min="5" max="5" width="21.36328125" customWidth="1"/>
-    <col min="8" max="8" width="18.08984375" customWidth="1"/>
-    <col min="9" max="9" width="14.36328125" customWidth="1"/>
-    <col min="10" max="10" width="18.26953125" customWidth="1"/>
+    <col min="1" max="1" width="40.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
@@ -30192,7 +30196,7 @@
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
     </row>
-    <row r="10" spans="1:8" ht="13">
+    <row r="10" spans="1:8" ht="13.2">
       <c r="A10" s="18" t="s">
         <v>155</v>
       </c>
@@ -30203,7 +30207,7 @@
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
     </row>
-    <row r="11" spans="1:8" ht="13">
+    <row r="11" spans="1:8" ht="13.2">
       <c r="A11" s="18" t="s">
         <v>157</v>
       </c>
@@ -30371,7 +30375,7 @@
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
     </row>
-    <row r="26" spans="1:10" ht="12.5">
+    <row r="26" spans="1:10" ht="13.2">
       <c r="A26" s="18" t="s">
         <v>187</v>
       </c>
@@ -30382,7 +30386,7 @@
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
     </row>
-    <row r="27" spans="1:10" ht="12.5">
+    <row r="27" spans="1:10" ht="13.2">
       <c r="A27" s="18" t="s">
         <v>189</v>
       </c>
@@ -30393,7 +30397,7 @@
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
     </row>
-    <row r="28" spans="1:10" ht="12.5">
+    <row r="28" spans="1:10" ht="13.2">
       <c r="A28" s="18" t="s">
         <v>191</v>
       </c>
@@ -30404,7 +30408,7 @@
       <c r="D28" s="18"/>
       <c r="E28" s="18"/>
     </row>
-    <row r="29" spans="1:10" ht="12.5">
+    <row r="29" spans="1:10" ht="13.2">
       <c r="A29" s="18" t="s">
         <v>193</v>
       </c>
@@ -30415,7 +30419,7 @@
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
     </row>
-    <row r="30" spans="1:10" ht="12.5">
+    <row r="30" spans="1:10" ht="13.2">
       <c r="A30" s="18" t="s">
         <v>195</v>
       </c>
@@ -30426,7 +30430,7 @@
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
     </row>
-    <row r="31" spans="1:10" ht="12.5">
+    <row r="31" spans="1:10" ht="13.2">
       <c r="A31" s="18" t="s">
         <v>197</v>
       </c>
@@ -30437,7 +30441,7 @@
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
     </row>
-    <row r="32" spans="1:10" ht="12.5">
+    <row r="32" spans="1:10" ht="13.2">
       <c r="A32" s="18" t="s">
         <v>199</v>
       </c>
@@ -30448,7 +30452,7 @@
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
     </row>
-    <row r="33" spans="1:5" ht="12.5">
+    <row r="33" spans="1:5" ht="13.2">
       <c r="A33" s="18" t="s">
         <v>201</v>
       </c>
@@ -30459,7 +30463,7 @@
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
     </row>
-    <row r="34" spans="1:5" ht="12.5">
+    <row r="34" spans="1:5" ht="13.2">
       <c r="A34" s="18" t="s">
         <v>203</v>
       </c>
@@ -30470,7 +30474,7 @@
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
     </row>
-    <row r="35" spans="1:5" ht="12.5">
+    <row r="35" spans="1:5" ht="13.2">
       <c r="A35" s="18" t="s">
         <v>205</v>
       </c>
@@ -30481,7 +30485,7 @@
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
     </row>
-    <row r="36" spans="1:5" ht="12.5">
+    <row r="36" spans="1:5" ht="13.2">
       <c r="A36" s="18" t="s">
         <v>207</v>
       </c>
@@ -30492,7 +30496,7 @@
       <c r="D36" s="18"/>
       <c r="E36" s="18"/>
     </row>
-    <row r="37" spans="1:5" ht="12.5">
+    <row r="37" spans="1:5" ht="13.2">
       <c r="A37" s="18" t="s">
         <v>209</v>
       </c>
@@ -30503,7 +30507,7 @@
       <c r="D37" s="18"/>
       <c r="E37" s="18"/>
     </row>
-    <row r="38" spans="1:5" ht="12.5">
+    <row r="38" spans="1:5" ht="13.2">
       <c r="A38" s="18" t="s">
         <v>211</v>
       </c>
@@ -30514,7 +30518,7 @@
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
     </row>
-    <row r="39" spans="1:5" ht="12.5">
+    <row r="39" spans="1:5" ht="13.2">
       <c r="A39" s="18" t="s">
         <v>213</v>
       </c>
@@ -30525,7 +30529,7 @@
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
     </row>
-    <row r="40" spans="1:5" ht="12.5">
+    <row r="40" spans="1:5" ht="13.2">
       <c r="A40" s="18" t="s">
         <v>21</v>
       </c>
@@ -30536,7 +30540,7 @@
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
     </row>
-    <row r="41" spans="1:5" ht="12.5">
+    <row r="41" spans="1:5" ht="13.2">
       <c r="A41" s="18" t="s">
         <v>216</v>
       </c>
@@ -30547,7 +30551,7 @@
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
     </row>
-    <row r="42" spans="1:5" ht="12.5">
+    <row r="42" spans="1:5" ht="13.2">
       <c r="A42" s="18" t="s">
         <v>218</v>
       </c>
@@ -30558,7 +30562,7 @@
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
     </row>
-    <row r="43" spans="1:5" ht="12.5">
+    <row r="43" spans="1:5" ht="13.2">
       <c r="A43" s="18" t="s">
         <v>220</v>
       </c>
@@ -30569,7 +30573,7 @@
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
     </row>
-    <row r="44" spans="1:5" ht="12.5">
+    <row r="44" spans="1:5" ht="13.2">
       <c r="A44" s="18" t="s">
         <v>222</v>
       </c>
@@ -30580,7 +30584,7 @@
       <c r="D44" s="18"/>
       <c r="E44" s="18"/>
     </row>
-    <row r="45" spans="1:5" ht="12.5">
+    <row r="45" spans="1:5" ht="13.2">
       <c r="A45" s="18" t="s">
         <v>224</v>
       </c>
@@ -30591,7 +30595,7 @@
       <c r="D45" s="18"/>
       <c r="E45" s="18"/>
     </row>
-    <row r="46" spans="1:5" ht="12.5">
+    <row r="46" spans="1:5" ht="13.2">
       <c r="A46" s="18" t="s">
         <v>226</v>
       </c>
@@ -30602,7 +30606,7 @@
       <c r="D46" s="18"/>
       <c r="E46" s="18"/>
     </row>
-    <row r="47" spans="1:5" ht="12.5">
+    <row r="47" spans="1:5" ht="13.2">
       <c r="A47" s="18" t="s">
         <v>228</v>
       </c>
@@ -30613,7 +30617,7 @@
       <c r="D47" s="18"/>
       <c r="E47" s="18"/>
     </row>
-    <row r="48" spans="1:5" ht="12.5">
+    <row r="48" spans="1:5" ht="13.2">
       <c r="A48" s="18" t="s">
         <v>230</v>
       </c>
@@ -30624,7 +30628,7 @@
       <c r="D48" s="18"/>
       <c r="E48" s="18"/>
     </row>
-    <row r="49" spans="1:5" ht="12.5">
+    <row r="49" spans="1:5" ht="13.2">
       <c r="A49" s="18" t="s">
         <v>232</v>
       </c>
@@ -30635,7 +30639,7 @@
       <c r="D49" s="18"/>
       <c r="E49" s="18"/>
     </row>
-    <row r="50" spans="1:5" ht="12.5">
+    <row r="50" spans="1:5" ht="13.2">
       <c r="A50" s="18" t="s">
         <v>234</v>
       </c>
@@ -30646,7 +30650,7 @@
       <c r="D50" s="18"/>
       <c r="E50" s="18"/>
     </row>
-    <row r="51" spans="1:5" ht="12.5">
+    <row r="51" spans="1:5" ht="13.2">
       <c r="A51" s="18" t="s">
         <v>236</v>
       </c>
@@ -30657,7 +30661,7 @@
       <c r="D51" s="18"/>
       <c r="E51" s="18"/>
     </row>
-    <row r="52" spans="1:5" ht="12.5">
+    <row r="52" spans="1:5" ht="13.2">
       <c r="A52" s="18" t="s">
         <v>238</v>
       </c>
@@ -30668,7 +30672,7 @@
       <c r="D52" s="18"/>
       <c r="E52" s="18"/>
     </row>
-    <row r="53" spans="1:5" ht="12.5">
+    <row r="53" spans="1:5" ht="13.2">
       <c r="A53" s="18" t="s">
         <v>240</v>
       </c>
@@ -30679,7 +30683,7 @@
       <c r="D53" s="18"/>
       <c r="E53" s="18"/>
     </row>
-    <row r="54" spans="1:5" ht="12.5">
+    <row r="54" spans="1:5" ht="13.2">
       <c r="A54" s="18" t="s">
         <v>242</v>
       </c>
@@ -30690,7 +30694,7 @@
       <c r="D54" s="18"/>
       <c r="E54" s="18"/>
     </row>
-    <row r="55" spans="1:5" ht="12.5">
+    <row r="55" spans="1:5" ht="13.2">
       <c r="A55" s="18" t="s">
         <v>244</v>
       </c>
@@ -30701,7 +30705,7 @@
       <c r="D55" s="18"/>
       <c r="E55" s="18"/>
     </row>
-    <row r="56" spans="1:5" ht="12.5">
+    <row r="56" spans="1:5" ht="13.2">
       <c r="A56" s="18" t="s">
         <v>246</v>
       </c>
@@ -30712,7 +30716,7 @@
       <c r="D56" s="18"/>
       <c r="E56" s="18"/>
     </row>
-    <row r="57" spans="1:5" ht="12.5">
+    <row r="57" spans="1:5" ht="13.2">
       <c r="A57" s="18" t="s">
         <v>248</v>
       </c>
@@ -30723,7 +30727,7 @@
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
     </row>
-    <row r="58" spans="1:5" ht="12.5">
+    <row r="58" spans="1:5" ht="13.2">
       <c r="A58" s="18" t="s">
         <v>250</v>
       </c>
@@ -30734,7 +30738,7 @@
       <c r="D58" s="18"/>
       <c r="E58" s="18"/>
     </row>
-    <row r="59" spans="1:5" ht="12.5">
+    <row r="59" spans="1:5" ht="13.2">
       <c r="A59" s="18" t="s">
         <v>252</v>
       </c>
@@ -30745,7 +30749,7 @@
       <c r="D59" s="18"/>
       <c r="E59" s="18"/>
     </row>
-    <row r="60" spans="1:5" ht="12.5">
+    <row r="60" spans="1:5" ht="13.2">
       <c r="A60" s="18" t="s">
         <v>254</v>
       </c>
@@ -30756,7 +30760,7 @@
       <c r="D60" s="18"/>
       <c r="E60" s="18"/>
     </row>
-    <row r="61" spans="1:5" ht="12.5">
+    <row r="61" spans="1:5" ht="13.2">
       <c r="A61" s="18" t="s">
         <v>256</v>
       </c>
@@ -30767,7 +30771,7 @@
       <c r="D61" s="18"/>
       <c r="E61" s="18"/>
     </row>
-    <row r="62" spans="1:5" ht="12.5">
+    <row r="62" spans="1:5" ht="13.2">
       <c r="A62" s="18" t="s">
         <v>258</v>
       </c>
@@ -30778,7 +30782,7 @@
       <c r="D62" s="18"/>
       <c r="E62" s="18"/>
     </row>
-    <row r="63" spans="1:5" ht="12.5">
+    <row r="63" spans="1:5" ht="13.2">
       <c r="A63" s="18" t="s">
         <v>260</v>
       </c>
@@ -30789,7 +30793,7 @@
       <c r="D63" s="18"/>
       <c r="E63" s="18"/>
     </row>
-    <row r="64" spans="1:5" ht="12.5">
+    <row r="64" spans="1:5" ht="13.2">
       <c r="A64" s="18" t="s">
         <v>262</v>
       </c>
@@ -30800,7 +30804,7 @@
       <c r="D64" s="18"/>
       <c r="E64" s="18"/>
     </row>
-    <row r="65" spans="1:5" ht="12.5">
+    <row r="65" spans="1:5" ht="13.2">
       <c r="A65" s="18" t="s">
         <v>264</v>
       </c>
@@ -30811,7 +30815,7 @@
       <c r="D65" s="18"/>
       <c r="E65" s="18"/>
     </row>
-    <row r="66" spans="1:5" ht="12.5">
+    <row r="66" spans="1:5" ht="13.2">
       <c r="A66" s="18" t="s">
         <v>266</v>
       </c>
@@ -30822,7 +30826,7 @@
       <c r="D66" s="18"/>
       <c r="E66" s="18"/>
     </row>
-    <row r="67" spans="1:5" ht="12.5">
+    <row r="67" spans="1:5" ht="13.2">
       <c r="A67" s="18" t="s">
         <v>268</v>
       </c>
@@ -30833,7 +30837,7 @@
       <c r="D67" s="18"/>
       <c r="E67" s="18"/>
     </row>
-    <row r="68" spans="1:5" ht="12.5">
+    <row r="68" spans="1:5" ht="13.2">
       <c r="A68" s="18" t="s">
         <v>270</v>
       </c>
@@ -30844,7 +30848,7 @@
       <c r="D68" s="18"/>
       <c r="E68" s="18"/>
     </row>
-    <row r="69" spans="1:5" ht="12.5">
+    <row r="69" spans="1:5" ht="13.2">
       <c r="A69" s="18" t="s">
         <v>272</v>
       </c>
@@ -30855,7 +30859,7 @@
       <c r="D69" s="18"/>
       <c r="E69" s="18"/>
     </row>
-    <row r="70" spans="1:5" ht="12.5">
+    <row r="70" spans="1:5" ht="13.2">
       <c r="A70" s="18" t="s">
         <v>274</v>
       </c>
@@ -30866,7 +30870,7 @@
       <c r="D70" s="18"/>
       <c r="E70" s="18"/>
     </row>
-    <row r="71" spans="1:5" ht="12.5">
+    <row r="71" spans="1:5" ht="13.2">
       <c r="A71" s="18" t="s">
         <v>276</v>
       </c>
@@ -30877,7 +30881,7 @@
       <c r="D71" s="18"/>
       <c r="E71" s="18"/>
     </row>
-    <row r="72" spans="1:5" ht="12.5">
+    <row r="72" spans="1:5" ht="13.2">
       <c r="A72" s="18" t="s">
         <v>278</v>
       </c>
@@ -30888,7 +30892,7 @@
       <c r="D72" s="18"/>
       <c r="E72" s="18"/>
     </row>
-    <row r="73" spans="1:5" ht="12.5">
+    <row r="73" spans="1:5" ht="13.2">
       <c r="A73" s="18" t="s">
         <v>280</v>
       </c>
@@ -30899,7 +30903,7 @@
       <c r="D73" s="18"/>
       <c r="E73" s="18"/>
     </row>
-    <row r="74" spans="1:5" ht="12.5">
+    <row r="74" spans="1:5" ht="13.2">
       <c r="A74" s="18" t="s">
         <v>282</v>
       </c>
@@ -30910,7 +30914,7 @@
       <c r="D74" s="18"/>
       <c r="E74" s="18"/>
     </row>
-    <row r="75" spans="1:5" ht="12.5">
+    <row r="75" spans="1:5" ht="13.2">
       <c r="A75" s="18" t="s">
         <v>284</v>
       </c>
@@ -30921,7 +30925,7 @@
       <c r="D75" s="18"/>
       <c r="E75" s="18"/>
     </row>
-    <row r="76" spans="1:5" ht="12.5">
+    <row r="76" spans="1:5" ht="13.2">
       <c r="A76" s="18" t="s">
         <v>286</v>
       </c>
@@ -30932,7 +30936,7 @@
       <c r="D76" s="18"/>
       <c r="E76" s="18"/>
     </row>
-    <row r="77" spans="1:5" ht="12.5">
+    <row r="77" spans="1:5" ht="13.2">
       <c r="A77" s="18"/>
       <c r="B77" s="18" t="s">
         <v>288</v>
@@ -30941,7 +30945,7 @@
       <c r="D77" s="18"/>
       <c r="E77" s="18"/>
     </row>
-    <row r="78" spans="1:5" ht="12.5">
+    <row r="78" spans="1:5" ht="13.2">
       <c r="A78" s="18"/>
       <c r="B78" s="18" t="s">
         <v>289</v>
@@ -30950,7 +30954,7 @@
       <c r="D78" s="18"/>
       <c r="E78" s="18"/>
     </row>
-    <row r="79" spans="1:5" ht="12.5">
+    <row r="79" spans="1:5" ht="13.2">
       <c r="A79" s="18"/>
       <c r="B79" s="18" t="s">
         <v>290</v>
@@ -30959,7 +30963,7 @@
       <c r="D79" s="18"/>
       <c r="E79" s="18"/>
     </row>
-    <row r="80" spans="1:5" ht="12.5">
+    <row r="80" spans="1:5" ht="13.2">
       <c r="A80" s="18"/>
       <c r="B80" s="18" t="s">
         <v>291</v>
@@ -30968,7 +30972,7 @@
       <c r="D80" s="18"/>
       <c r="E80" s="18"/>
     </row>
-    <row r="81" spans="1:5" ht="12.5">
+    <row r="81" spans="1:5" ht="13.2">
       <c r="A81" s="18"/>
       <c r="B81" s="18" t="s">
         <v>292</v>
@@ -30977,7 +30981,7 @@
       <c r="D81" s="18"/>
       <c r="E81" s="18"/>
     </row>
-    <row r="82" spans="1:5" ht="12.5">
+    <row r="82" spans="1:5" ht="13.2">
       <c r="A82" s="18"/>
       <c r="B82" s="18" t="s">
         <v>293</v>
@@ -30986,7 +30990,7 @@
       <c r="D82" s="18"/>
       <c r="E82" s="18"/>
     </row>
-    <row r="83" spans="1:5" ht="12.5">
+    <row r="83" spans="1:5" ht="13.2">
       <c r="A83" s="18"/>
       <c r="B83" s="18" t="s">
         <v>294</v>
@@ -30995,7 +30999,7 @@
       <c r="D83" s="18"/>
       <c r="E83" s="18"/>
     </row>
-    <row r="84" spans="1:5" ht="12.5">
+    <row r="84" spans="1:5" ht="13.2">
       <c r="A84" s="18"/>
       <c r="B84" s="18" t="s">
         <v>295</v>
@@ -31004,7 +31008,7 @@
       <c r="D84" s="18"/>
       <c r="E84" s="18"/>
     </row>
-    <row r="85" spans="1:5" ht="12.5">
+    <row r="85" spans="1:5" ht="13.2">
       <c r="A85" s="18"/>
       <c r="B85" s="18" t="s">
         <v>296</v>
@@ -31013,7 +31017,7 @@
       <c r="D85" s="18"/>
       <c r="E85" s="18"/>
     </row>
-    <row r="86" spans="1:5" ht="12.5">
+    <row r="86" spans="1:5" ht="13.2">
       <c r="A86" s="18"/>
       <c r="B86" s="18" t="s">
         <v>297</v>
@@ -31022,7 +31026,7 @@
       <c r="D86" s="18"/>
       <c r="E86" s="18"/>
     </row>
-    <row r="87" spans="1:5" ht="12.5">
+    <row r="87" spans="1:5" ht="13.2">
       <c r="A87" s="18"/>
       <c r="B87" s="18" t="s">
         <v>298</v>
@@ -31031,7 +31035,7 @@
       <c r="D87" s="18"/>
       <c r="E87" s="18"/>
     </row>
-    <row r="88" spans="1:5" ht="12.5">
+    <row r="88" spans="1:5" ht="13.2">
       <c r="A88" s="18"/>
       <c r="B88" s="18" t="s">
         <v>299</v>
@@ -31040,7 +31044,7 @@
       <c r="D88" s="18"/>
       <c r="E88" s="18"/>
     </row>
-    <row r="89" spans="1:5" ht="12.5">
+    <row r="89" spans="1:5" ht="13.2">
       <c r="A89" s="18"/>
       <c r="B89" s="18" t="s">
         <v>300</v>
@@ -31049,7 +31053,7 @@
       <c r="D89" s="18"/>
       <c r="E89" s="18"/>
     </row>
-    <row r="90" spans="1:5" ht="12.5">
+    <row r="90" spans="1:5" ht="13.2">
       <c r="A90" s="18"/>
       <c r="B90" s="18" t="s">
         <v>301</v>
@@ -31073,19 +31077,19 @@
   </sheetPr>
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.90625" customWidth="1"/>
-    <col min="2" max="2" width="33.6328125" customWidth="1"/>
-    <col min="3" max="3" width="30.26953125" customWidth="1"/>
-    <col min="4" max="4" width="19.90625" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.21875" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="35">
+    <row r="1" spans="1:4" ht="34.799999999999997">
       <c r="A1" s="28" t="s">
         <v>302</v>
       </c>
@@ -31353,7 +31357,7 @@
       <c r="C25" s="18"/>
       <c r="D25" s="18"/>
     </row>
-    <row r="26" spans="1:4" ht="12.5">
+    <row r="26" spans="1:4" ht="13.2">
       <c r="A26" s="18" t="s">
         <v>339</v>
       </c>
@@ -31363,7 +31367,7 @@
       <c r="C26" s="18"/>
       <c r="D26" s="18"/>
     </row>
-    <row r="27" spans="1:4" ht="12.5">
+    <row r="27" spans="1:4" ht="13.2">
       <c r="A27" s="18" t="s">
         <v>340</v>
       </c>
@@ -31373,7 +31377,7 @@
       <c r="C27" s="18"/>
       <c r="D27" s="18"/>
     </row>
-    <row r="28" spans="1:4" ht="12.5">
+    <row r="28" spans="1:4" ht="13.2">
       <c r="A28" s="18" t="s">
         <v>341</v>
       </c>
@@ -31383,7 +31387,7 @@
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
     </row>
-    <row r="29" spans="1:4" ht="12.5">
+    <row r="29" spans="1:4" ht="13.2">
       <c r="A29" s="18" t="s">
         <v>343</v>
       </c>
@@ -31393,7 +31397,7 @@
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
     </row>
-    <row r="30" spans="1:4" ht="12.5">
+    <row r="30" spans="1:4" ht="13.2">
       <c r="A30" s="18" t="s">
         <v>344</v>
       </c>
@@ -31403,7 +31407,7 @@
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
     </row>
-    <row r="31" spans="1:4" ht="12.5">
+    <row r="31" spans="1:4" ht="13.2">
       <c r="A31" s="18" t="s">
         <v>345</v>
       </c>
@@ -31413,7 +31417,7 @@
       <c r="C31" s="18"/>
       <c r="D31" s="18"/>
     </row>
-    <row r="32" spans="1:4" ht="12.5">
+    <row r="32" spans="1:4" ht="13.2">
       <c r="A32" s="18" t="s">
         <v>346</v>
       </c>
@@ -31423,7 +31427,7 @@
       <c r="C32" s="18"/>
       <c r="D32" s="18"/>
     </row>
-    <row r="33" spans="1:4" ht="12.5">
+    <row r="33" spans="1:4" ht="13.2">
       <c r="A33" s="18" t="s">
         <v>348</v>
       </c>
@@ -31433,7 +31437,7 @@
       <c r="C33" s="18"/>
       <c r="D33" s="18"/>
     </row>
-    <row r="34" spans="1:4" ht="12.5">
+    <row r="34" spans="1:4" ht="13.2">
       <c r="A34" s="18" t="s">
         <v>350</v>
       </c>
@@ -31443,7 +31447,7 @@
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
     </row>
-    <row r="35" spans="1:4" ht="12.5">
+    <row r="35" spans="1:4" ht="13.2">
       <c r="A35" s="18" t="s">
         <v>352</v>
       </c>
@@ -31451,7 +31455,7 @@
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
     </row>
-    <row r="36" spans="1:4" ht="12.5">
+    <row r="36" spans="1:4" ht="13.2">
       <c r="A36" s="18" t="s">
         <v>353</v>
       </c>
@@ -31459,7 +31463,7 @@
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
     </row>
-    <row r="37" spans="1:4" ht="12.5">
+    <row r="37" spans="1:4" ht="13.2">
       <c r="A37" s="18" t="s">
         <v>354</v>
       </c>
@@ -31467,7 +31471,7 @@
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
     </row>
-    <row r="38" spans="1:4" ht="12.5">
+    <row r="38" spans="1:4" ht="13.2">
       <c r="A38" s="18" t="s">
         <v>355</v>
       </c>
@@ -31475,7 +31479,7 @@
       <c r="C38" s="18"/>
       <c r="D38" s="18"/>
     </row>
-    <row r="39" spans="1:4" ht="12.5">
+    <row r="39" spans="1:4" ht="13.2">
       <c r="A39" s="18" t="s">
         <v>356</v>
       </c>
@@ -31483,7 +31487,7 @@
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
     </row>
-    <row r="40" spans="1:4" ht="12.5">
+    <row r="40" spans="1:4" ht="13.2">
       <c r="A40" s="18" t="s">
         <v>265</v>
       </c>
@@ -31491,7 +31495,7 @@
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
     </row>
-    <row r="41" spans="1:4" ht="12.5">
+    <row r="41" spans="1:4" ht="13.2">
       <c r="A41" s="18" t="s">
         <v>259</v>
       </c>
@@ -31499,7 +31503,7 @@
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
     </row>
-    <row r="42" spans="1:4" ht="12.5">
+    <row r="42" spans="1:4" ht="13.2">
       <c r="A42" s="18" t="s">
         <v>357</v>
       </c>
@@ -31507,7 +31511,7 @@
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
     </row>
-    <row r="43" spans="1:4" ht="12.5">
+    <row r="43" spans="1:4" ht="13.2">
       <c r="A43" s="18" t="s">
         <v>358</v>
       </c>
@@ -31515,7 +31519,7 @@
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
     </row>
-    <row r="44" spans="1:4" ht="12.5">
+    <row r="44" spans="1:4" ht="13.2">
       <c r="A44" s="18" t="s">
         <v>359</v>
       </c>
@@ -31523,7 +31527,7 @@
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
     </row>
-    <row r="45" spans="1:4" ht="12.5">
+    <row r="45" spans="1:4" ht="13.2">
       <c r="A45" s="18" t="s">
         <v>198</v>
       </c>
@@ -31531,7 +31535,7 @@
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
     </row>
-    <row r="46" spans="1:4" ht="12.5">
+    <row r="46" spans="1:4" ht="13.2">
       <c r="A46" s="18" t="s">
         <v>200</v>
       </c>
@@ -31539,7 +31543,7 @@
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
     </row>
-    <row r="47" spans="1:4" ht="12.5">
+    <row r="47" spans="1:4" ht="13.2">
       <c r="A47" s="18" t="s">
         <v>202</v>
       </c>
@@ -31547,7 +31551,7 @@
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
     </row>
-    <row r="48" spans="1:4" ht="12.5">
+    <row r="48" spans="1:4" ht="13.2">
       <c r="A48" s="18" t="s">
         <v>204</v>
       </c>
@@ -31555,7 +31559,7 @@
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
     </row>
-    <row r="49" spans="1:4" ht="12.5">
+    <row r="49" spans="1:4" ht="13.2">
       <c r="A49" s="18" t="s">
         <v>206</v>
       </c>
@@ -31563,7 +31567,7 @@
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
     </row>
-    <row r="50" spans="1:4" ht="12.5">
+    <row r="50" spans="1:4" ht="13.2">
       <c r="A50" s="18" t="s">
         <v>208</v>
       </c>
@@ -31571,7 +31575,7 @@
       <c r="C50" s="18"/>
       <c r="D50" s="18"/>
     </row>
-    <row r="51" spans="1:4" ht="12.5">
+    <row r="51" spans="1:4" ht="13.2">
       <c r="A51" s="18" t="s">
         <v>210</v>
       </c>
@@ -31579,7 +31583,7 @@
       <c r="C51" s="18"/>
       <c r="D51" s="18"/>
     </row>
-    <row r="52" spans="1:4" ht="12.5">
+    <row r="52" spans="1:4" ht="13.2">
       <c r="A52" s="18" t="s">
         <v>212</v>
       </c>
@@ -31587,7 +31591,7 @@
       <c r="C52" s="18"/>
       <c r="D52" s="18"/>
     </row>
-    <row r="53" spans="1:4" ht="12.5">
+    <row r="53" spans="1:4" ht="13.2">
       <c r="A53" s="18" t="s">
         <v>214</v>
       </c>
@@ -31595,7 +31599,7 @@
       <c r="C53" s="18"/>
       <c r="D53" s="18"/>
     </row>
-    <row r="54" spans="1:4" ht="12.5">
+    <row r="54" spans="1:4" ht="13.2">
       <c r="A54" s="18" t="s">
         <v>217</v>
       </c>
@@ -31603,7 +31607,7 @@
       <c r="C54" s="18"/>
       <c r="D54" s="18"/>
     </row>
-    <row r="55" spans="1:4" ht="12.5">
+    <row r="55" spans="1:4" ht="13.2">
       <c r="A55" s="18" t="s">
         <v>219</v>
       </c>
@@ -31611,7 +31615,7 @@
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
     </row>
-    <row r="56" spans="1:4" ht="12.5">
+    <row r="56" spans="1:4" ht="13.2">
       <c r="A56" s="18" t="s">
         <v>221</v>
       </c>
@@ -31619,7 +31623,7 @@
       <c r="C56" s="18"/>
       <c r="D56" s="18"/>
     </row>
-    <row r="57" spans="1:4" ht="12.5">
+    <row r="57" spans="1:4" ht="13.2">
       <c r="A57" s="18" t="s">
         <v>223</v>
       </c>
@@ -31627,7 +31631,7 @@
       <c r="C57" s="18"/>
       <c r="D57" s="18"/>
     </row>
-    <row r="58" spans="1:4" ht="12.5">
+    <row r="58" spans="1:4" ht="13.2">
       <c r="A58" s="18" t="s">
         <v>225</v>
       </c>
@@ -31635,7 +31639,7 @@
       <c r="C58" s="18"/>
       <c r="D58" s="18"/>
     </row>
-    <row r="59" spans="1:4" ht="12.5">
+    <row r="59" spans="1:4" ht="13.2">
       <c r="A59" s="18" t="s">
         <v>174</v>
       </c>
@@ -31643,7 +31647,7 @@
       <c r="C59" s="18"/>
       <c r="D59" s="18"/>
     </row>
-    <row r="60" spans="1:4" ht="12.5">
+    <row r="60" spans="1:4" ht="13.2">
       <c r="A60" s="18" t="s">
         <v>176</v>
       </c>
@@ -31651,7 +31655,7 @@
       <c r="C60" s="18"/>
       <c r="D60" s="18"/>
     </row>
-    <row r="61" spans="1:4" ht="12.5">
+    <row r="61" spans="1:4" ht="13.2">
       <c r="A61" s="18" t="s">
         <v>178</v>
       </c>
@@ -31659,7 +31663,7 @@
       <c r="C61" s="18"/>
       <c r="D61" s="18"/>
     </row>
-    <row r="62" spans="1:4" ht="12.5">
+    <row r="62" spans="1:4" ht="13.2">
       <c r="A62" s="18" t="s">
         <v>180</v>
       </c>
@@ -31667,7 +31671,7 @@
       <c r="C62" s="18"/>
       <c r="D62" s="18"/>
     </row>
-    <row r="63" spans="1:4" ht="12.5">
+    <row r="63" spans="1:4" ht="13.2">
       <c r="A63" s="18" t="s">
         <v>182</v>
       </c>
@@ -31675,7 +31679,7 @@
       <c r="C63" s="18"/>
       <c r="D63" s="18"/>
     </row>
-    <row r="64" spans="1:4" ht="12.5">
+    <row r="64" spans="1:4" ht="13.2">
       <c r="A64" s="18" t="s">
         <v>184</v>
       </c>
@@ -31683,7 +31687,7 @@
       <c r="C64" s="18"/>
       <c r="D64" s="18"/>
     </row>
-    <row r="65" spans="1:4" ht="12.5">
+    <row r="65" spans="1:4" ht="13.2">
       <c r="A65" s="18" t="s">
         <v>185</v>
       </c>
@@ -31691,7 +31695,7 @@
       <c r="C65" s="18"/>
       <c r="D65" s="18"/>
     </row>
-    <row r="66" spans="1:4" ht="12.5">
+    <row r="66" spans="1:4" ht="13.2">
       <c r="A66" s="18" t="s">
         <v>187</v>
       </c>
@@ -31699,7 +31703,7 @@
       <c r="C66" s="18"/>
       <c r="D66" s="18"/>
     </row>
-    <row r="67" spans="1:4" ht="12.5">
+    <row r="67" spans="1:4" ht="13.2">
       <c r="A67" s="18" t="s">
         <v>189</v>
       </c>
@@ -31707,7 +31711,7 @@
       <c r="C67" s="18"/>
       <c r="D67" s="18"/>
     </row>
-    <row r="68" spans="1:4" ht="12.5">
+    <row r="68" spans="1:4" ht="13.2">
       <c r="A68" s="18" t="s">
         <v>191</v>
       </c>
@@ -31715,7 +31719,7 @@
       <c r="C68" s="18"/>
       <c r="D68" s="18"/>
     </row>
-    <row r="69" spans="1:4" ht="12.5">
+    <row r="69" spans="1:4" ht="13.2">
       <c r="A69" s="18" t="s">
         <v>193</v>
       </c>
@@ -31723,7 +31727,7 @@
       <c r="C69" s="18"/>
       <c r="D69" s="18"/>
     </row>
-    <row r="70" spans="1:4" ht="12.5">
+    <row r="70" spans="1:4" ht="13.2">
       <c r="A70" s="18" t="s">
         <v>248</v>
       </c>
@@ -31731,7 +31735,7 @@
       <c r="C70" s="18"/>
       <c r="D70" s="18"/>
     </row>
-    <row r="71" spans="1:4" ht="12.5">
+    <row r="71" spans="1:4" ht="13.2">
       <c r="A71" s="18" t="s">
         <v>250</v>
       </c>
@@ -31739,7 +31743,7 @@
       <c r="C71" s="18"/>
       <c r="D71" s="18"/>
     </row>
-    <row r="72" spans="1:4" ht="12.5">
+    <row r="72" spans="1:4" ht="13.2">
       <c r="A72" s="18" t="s">
         <v>252</v>
       </c>
@@ -31747,7 +31751,7 @@
       <c r="C72" s="18"/>
       <c r="D72" s="18"/>
     </row>
-    <row r="73" spans="1:4" ht="12.5">
+    <row r="73" spans="1:4" ht="13.2">
       <c r="A73" s="18" t="s">
         <v>254</v>
       </c>
@@ -31755,7 +31759,7 @@
       <c r="C73" s="18"/>
       <c r="D73" s="18"/>
     </row>
-    <row r="74" spans="1:4" ht="12.5">
+    <row r="74" spans="1:4" ht="13.2">
       <c r="A74" s="18" t="s">
         <v>256</v>
       </c>
@@ -31763,7 +31767,7 @@
       <c r="C74" s="18"/>
       <c r="D74" s="18"/>
     </row>
-    <row r="75" spans="1:4" ht="12.5">
+    <row r="75" spans="1:4" ht="13.2">
       <c r="A75" s="18" t="s">
         <v>258</v>
       </c>
@@ -31771,7 +31775,7 @@
       <c r="C75" s="18"/>
       <c r="D75" s="18"/>
     </row>
-    <row r="76" spans="1:4" ht="12.5">
+    <row r="76" spans="1:4" ht="13.2">
       <c r="A76" s="18" t="s">
         <v>260</v>
       </c>
@@ -31779,7 +31783,7 @@
       <c r="C76" s="18"/>
       <c r="D76" s="18"/>
     </row>
-    <row r="77" spans="1:4" ht="12.5">
+    <row r="77" spans="1:4" ht="13.2">
       <c r="A77" s="18" t="s">
         <v>360</v>
       </c>
@@ -31787,7 +31791,7 @@
       <c r="C77" s="18"/>
       <c r="D77" s="18"/>
     </row>
-    <row r="78" spans="1:4" ht="12.5">
+    <row r="78" spans="1:4" ht="13.2">
       <c r="A78" s="18" t="s">
         <v>264</v>
       </c>
@@ -31795,7 +31799,7 @@
       <c r="C78" s="18"/>
       <c r="D78" s="18"/>
     </row>
-    <row r="79" spans="1:4" ht="12.5">
+    <row r="79" spans="1:4" ht="13.2">
       <c r="A79" s="18" t="s">
         <v>266</v>
       </c>
@@ -31803,7 +31807,7 @@
       <c r="C79" s="18"/>
       <c r="D79" s="18"/>
     </row>
-    <row r="80" spans="1:4" ht="12.5">
+    <row r="80" spans="1:4" ht="13.2">
       <c r="A80" s="18" t="s">
         <v>268</v>
       </c>
@@ -31811,7 +31815,7 @@
       <c r="C80" s="18"/>
       <c r="D80" s="18"/>
     </row>
-    <row r="81" spans="1:4" ht="12.5">
+    <row r="81" spans="1:4" ht="13.2">
       <c r="A81" s="18" t="s">
         <v>270</v>
       </c>
@@ -31819,7 +31823,7 @@
       <c r="C81" s="18"/>
       <c r="D81" s="18"/>
     </row>
-    <row r="82" spans="1:4" ht="12.5">
+    <row r="82" spans="1:4" ht="13.2">
       <c r="A82" s="18" t="s">
         <v>272</v>
       </c>
@@ -31827,7 +31831,7 @@
       <c r="C82" s="18"/>
       <c r="D82" s="18"/>
     </row>
-    <row r="83" spans="1:4" ht="12.5">
+    <row r="83" spans="1:4" ht="13.2">
       <c r="A83" s="18" t="s">
         <v>274</v>
       </c>
@@ -31835,7 +31839,7 @@
       <c r="C83" s="18"/>
       <c r="D83" s="18"/>
     </row>
-    <row r="84" spans="1:4" ht="12.5">
+    <row r="84" spans="1:4" ht="13.2">
       <c r="A84" s="18" t="s">
         <v>276</v>
       </c>
@@ -31843,7 +31847,7 @@
       <c r="C84" s="18"/>
       <c r="D84" s="18"/>
     </row>
-    <row r="85" spans="1:4" ht="12.5">
+    <row r="85" spans="1:4" ht="13.2">
       <c r="A85" s="18" t="s">
         <v>278</v>
       </c>
@@ -31851,7 +31855,7 @@
       <c r="C85" s="18"/>
       <c r="D85" s="18"/>
     </row>
-    <row r="86" spans="1:4" ht="12.5">
+    <row r="86" spans="1:4" ht="13.2">
       <c r="A86" s="18" t="s">
         <v>280</v>
       </c>
@@ -31859,7 +31863,7 @@
       <c r="C86" s="18"/>
       <c r="D86" s="18"/>
     </row>
-    <row r="87" spans="1:4" ht="12.5">
+    <row r="87" spans="1:4" ht="13.2">
       <c r="A87" s="18" t="s">
         <v>282</v>
       </c>
@@ -31867,7 +31871,7 @@
       <c r="C87" s="18"/>
       <c r="D87" s="18"/>
     </row>
-    <row r="88" spans="1:4" ht="12.5">
+    <row r="88" spans="1:4" ht="13.2">
       <c r="A88" s="18" t="s">
         <v>284</v>
       </c>
@@ -31875,7 +31879,7 @@
       <c r="C88" s="18"/>
       <c r="D88" s="18"/>
     </row>
-    <row r="89" spans="1:4" ht="12.5">
+    <row r="89" spans="1:4" ht="13.2">
       <c r="A89" s="18" t="s">
         <v>286</v>
       </c>
@@ -31883,7 +31887,7 @@
       <c r="C89" s="18"/>
       <c r="D89" s="18"/>
     </row>
-    <row r="90" spans="1:4" ht="12.5">
+    <row r="90" spans="1:4" ht="13.2">
       <c r="A90" s="18" t="s">
         <v>361</v>
       </c>
@@ -31891,7 +31895,7 @@
       <c r="C90" s="18"/>
       <c r="D90" s="18"/>
     </row>
-    <row r="91" spans="1:4" ht="12.5">
+    <row r="91" spans="1:4" ht="13.2">
       <c r="A91" s="18" t="s">
         <v>357</v>
       </c>
@@ -31899,7 +31903,7 @@
       <c r="C91" s="18"/>
       <c r="D91" s="18"/>
     </row>
-    <row r="92" spans="1:4" ht="12.5">
+    <row r="92" spans="1:4" ht="13.2">
       <c r="A92" s="18" t="s">
         <v>362</v>
       </c>
@@ -31907,7 +31911,7 @@
       <c r="C92" s="18"/>
       <c r="D92" s="18"/>
     </row>
-    <row r="93" spans="1:4" ht="12.5">
+    <row r="93" spans="1:4" ht="13.2">
       <c r="A93" s="18"/>
       <c r="B93" s="18"/>
       <c r="C93" s="18"/>
@@ -31932,7 +31936,7 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
   </cols>

</xml_diff>